<commit_message>
Own model for 2014, 2015 and 2016
Now the codeis performing the L-K model for 2014 and 2015 using the respectively SUT Eurostat Database and the relative GDP in M€@2016. After that all the other years are run using the structure of 2016.
</commit_message>
<xml_diff>
--- a/Database/Italy_2016_SUT.xlsx
+++ b/Database/Italy_2016_SUT.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gollinucci\Documents\GitHub\COVID2030\Database\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD95DA5F-6ED1-4881-B5E6-730B169FCC34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4170" yWindow="-21720" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4170" yWindow="-21720" windowWidth="38640" windowHeight="21240"/>
   </bookViews>
   <sheets>
     <sheet name="SUT" sheetId="1" r:id="rId1"/>
@@ -614,7 +608,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#.0#############E+###"/>
     <numFmt numFmtId="165" formatCode="0;\-;\-"/>
@@ -682,7 +676,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -703,7 +697,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -745,7 +739,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -778,26 +772,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -830,23 +807,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1022,76 +982,76 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ER157"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="F124" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="6" topLeftCell="F54" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A144" sqref="A144"/>
+      <selection pane="bottomRight" activeCell="M77" sqref="M77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="18.77734375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="27.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
     <col min="7" max="9" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="23" width="9" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="25" max="31" width="9" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="9" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="36" max="40" width="9" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="42" max="49" width="9" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="51" max="59" width="9" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="61" max="61" width="9" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="63" max="64" width="9" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="66" max="67" width="10" bestFit="1" customWidth="1"/>
-    <col min="68" max="69" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="70" max="71" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="68" max="69" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="70" max="71" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="73" max="74" width="10" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="76" max="76" width="12" bestFit="1" customWidth="1"/>
-    <col min="77" max="89" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="77" max="89" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="90" max="90" width="12" bestFit="1" customWidth="1"/>
-    <col min="91" max="95" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="91" max="95" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="96" max="96" width="10" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="98" max="98" width="12" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="100" max="101" width="12" bestFit="1" customWidth="1"/>
-    <col min="102" max="105" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="102" max="105" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="106" max="106" width="10" bestFit="1" customWidth="1"/>
     <col min="107" max="107" width="12" bestFit="1" customWidth="1"/>
     <col min="108" max="108" width="10" bestFit="1" customWidth="1"/>
-    <col min="109" max="115" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="109" max="115" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="116" max="116" width="12" bestFit="1" customWidth="1"/>
-    <col min="117" max="122" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="117" max="122" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="123" max="123" width="10" bestFit="1" customWidth="1"/>
-    <col min="124" max="125" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="124" max="125" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="126" max="126" width="12" bestFit="1" customWidth="1"/>
-    <col min="127" max="127" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="127" max="127" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="128" max="128" width="12" bestFit="1" customWidth="1"/>
-    <col min="129" max="132" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="129" max="132" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="133" max="133" width="10" bestFit="1" customWidth="1"/>
-    <col min="134" max="135" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="134" max="135" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="136" max="136" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:139" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:139" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1503,7 +1463,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="str">
         <v>Sectors</v>
@@ -1911,7 +1871,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="3" spans="1:139" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:139" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="E3" s="1" t="str">
         <v>Macro Sectors</v>
@@ -2319,7 +2279,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="4" spans="1:139" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:139" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -2730,7 +2690,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="5" spans="1:139" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:139" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -3132,7 +3092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:139" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:139" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>166</v>
       </c>
@@ -3149,7 +3109,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="7" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
@@ -3565,7 +3525,7 @@
         <v>5726.1</v>
       </c>
     </row>
-    <row r="8" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>4</v>
       </c>
@@ -3981,7 +3941,7 @@
         <v>113.3</v>
       </c>
     </row>
-    <row r="9" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>4</v>
       </c>
@@ -4397,7 +4357,7 @@
         <v>224.9</v>
       </c>
     </row>
-    <row r="10" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>4</v>
       </c>
@@ -4813,7 +4773,7 @@
         <v>957.1</v>
       </c>
     </row>
-    <row r="11" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>4</v>
       </c>
@@ -5229,7 +5189,7 @@
         <v>31006.400000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>4</v>
       </c>
@@ -5645,7 +5605,7 @@
         <v>44034.5</v>
       </c>
     </row>
-    <row r="13" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>4</v>
       </c>
@@ -6061,7 +6021,7 @@
         <v>1693.2</v>
       </c>
     </row>
-    <row r="14" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>4</v>
       </c>
@@ -6477,7 +6437,7 @@
         <v>6530.8</v>
       </c>
     </row>
-    <row r="15" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
@@ -6893,7 +6853,7 @@
         <v>57.1</v>
       </c>
     </row>
-    <row r="16" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>4</v>
       </c>
@@ -7309,7 +7269,7 @@
         <v>10941.2</v>
       </c>
     </row>
-    <row r="17" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>4</v>
       </c>
@@ -7725,7 +7685,7 @@
         <v>25747.7</v>
       </c>
     </row>
-    <row r="18" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>4</v>
       </c>
@@ -8141,7 +8101,7 @@
         <v>15429.6</v>
       </c>
     </row>
-    <row r="19" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>4</v>
       </c>
@@ -8557,7 +8517,7 @@
         <v>14867.8</v>
       </c>
     </row>
-    <row r="20" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>4</v>
       </c>
@@ -8973,7 +8933,7 @@
         <v>9753.1</v>
       </c>
     </row>
-    <row r="21" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>4</v>
       </c>
@@ -9389,7 +9349,7 @@
         <v>23130</v>
       </c>
     </row>
-    <row r="22" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>4</v>
       </c>
@@ -9805,7 +9765,7 @@
         <v>18265.3</v>
       </c>
     </row>
-    <row r="23" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>4</v>
       </c>
@@ -10221,7 +10181,7 @@
         <v>12907.8</v>
       </c>
     </row>
-    <row r="24" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>4</v>
       </c>
@@ -10637,7 +10597,7 @@
         <v>21676</v>
       </c>
     </row>
-    <row r="25" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>4</v>
       </c>
@@ -11053,7 +11013,7 @@
         <v>75279.199999999997</v>
       </c>
     </row>
-    <row r="26" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>4</v>
       </c>
@@ -11469,7 +11429,7 @@
         <v>29850.9</v>
       </c>
     </row>
-    <row r="27" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>4</v>
       </c>
@@ -11885,7 +11845,7 @@
         <v>13218.1</v>
       </c>
     </row>
-    <row r="28" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>4</v>
       </c>
@@ -12301,7 +12261,7 @@
         <v>23116.5</v>
       </c>
     </row>
-    <row r="29" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>4</v>
       </c>
@@ -12717,7 +12677,7 @@
         <v>256.5</v>
       </c>
     </row>
-    <row r="30" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>4</v>
       </c>
@@ -13133,7 +13093,7 @@
         <v>351.4</v>
       </c>
     </row>
-    <row r="31" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>4</v>
       </c>
@@ -13549,7 +13509,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="32" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>4</v>
       </c>
@@ -13965,7 +13925,7 @@
         <v>1269.4000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>4</v>
       </c>
@@ -14381,7 +14341,7 @@
         <v>421.9</v>
       </c>
     </row>
-    <row r="34" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>4</v>
       </c>
@@ -14797,7 +14757,7 @@
         <v>4905.3999999999996</v>
       </c>
     </row>
-    <row r="35" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>4</v>
       </c>
@@ -15213,7 +15173,7 @@
         <v>9515.1</v>
       </c>
     </row>
-    <row r="36" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>4</v>
       </c>
@@ -15629,7 +15589,7 @@
         <v>7047.4</v>
       </c>
     </row>
-    <row r="37" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>4</v>
       </c>
@@ -16045,7 +16005,7 @@
         <v>3799</v>
       </c>
     </row>
-    <row r="38" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>4</v>
       </c>
@@ -16461,7 +16421,7 @@
         <v>2373.4</v>
       </c>
     </row>
-    <row r="39" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>4</v>
       </c>
@@ -16877,7 +16837,7 @@
         <v>1889.5</v>
       </c>
     </row>
-    <row r="40" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>4</v>
       </c>
@@ -17293,7 +17253,7 @@
         <v>7107</v>
       </c>
     </row>
-    <row r="41" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>4</v>
       </c>
@@ -17709,7 +17669,7 @@
         <v>608.5</v>
       </c>
     </row>
-    <row r="42" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>4</v>
       </c>
@@ -18125,7 +18085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>4</v>
       </c>
@@ -18541,7 +18501,7 @@
         <v>1400.1</v>
       </c>
     </row>
-    <row r="44" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>4</v>
       </c>
@@ -18957,7 +18917,7 @@
         <v>939.4</v>
       </c>
     </row>
-    <row r="45" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>4</v>
       </c>
@@ -19373,7 +19333,7 @@
         <v>3435.8</v>
       </c>
     </row>
-    <row r="46" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>4</v>
       </c>
@@ -19789,7 +19749,7 @@
         <v>3234.1</v>
       </c>
     </row>
-    <row r="47" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>4</v>
       </c>
@@ -20205,7 +20165,7 @@
         <v>2904.9</v>
       </c>
     </row>
-    <row r="48" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>4</v>
       </c>
@@ -20621,7 +20581,7 @@
         <v>1534</v>
       </c>
     </row>
-    <row r="49" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>4</v>
       </c>
@@ -21037,7 +20997,7 @@
         <v>2656.2</v>
       </c>
     </row>
-    <row r="50" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>4</v>
       </c>
@@ -21453,7 +21413,7 @@
         <v>938.7</v>
       </c>
     </row>
-    <row r="51" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>4</v>
       </c>
@@ -21869,7 +21829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>4</v>
       </c>
@@ -22285,7 +22245,7 @@
         <v>2522.8000000000002</v>
       </c>
     </row>
-    <row r="53" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>4</v>
       </c>
@@ -22701,7 +22661,7 @@
         <v>2341.1</v>
       </c>
     </row>
-    <row r="54" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>4</v>
       </c>
@@ -23117,7 +23077,7 @@
         <v>3019.6</v>
       </c>
     </row>
-    <row r="55" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>4</v>
       </c>
@@ -23533,7 +23493,7 @@
         <v>1557.5</v>
       </c>
     </row>
-    <row r="56" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>4</v>
       </c>
@@ -23949,7 +23909,7 @@
         <v>2447.8000000000002</v>
       </c>
     </row>
-    <row r="57" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>4</v>
       </c>
@@ -24365,7 +24325,7 @@
         <v>3463.4</v>
       </c>
     </row>
-    <row r="58" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>4</v>
       </c>
@@ -24781,7 +24741,7 @@
         <v>792.4</v>
       </c>
     </row>
-    <row r="59" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>4</v>
       </c>
@@ -25197,7 +25157,7 @@
         <v>924.5</v>
       </c>
     </row>
-    <row r="60" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>4</v>
       </c>
@@ -25613,7 +25573,7 @@
         <v>3404.1</v>
       </c>
     </row>
-    <row r="61" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
         <v>4</v>
       </c>
@@ -26029,7 +25989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
         <v>4</v>
       </c>
@@ -26445,7 +26405,7 @@
         <v>34.200000000000003</v>
       </c>
     </row>
-    <row r="63" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>4</v>
       </c>
@@ -26861,7 +26821,7 @@
         <v>17.3</v>
       </c>
     </row>
-    <row r="64" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>4</v>
       </c>
@@ -27277,7 +27237,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
         <v>4</v>
       </c>
@@ -27693,7 +27653,7 @@
         <v>346.6</v>
       </c>
     </row>
-    <row r="66" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
         <v>4</v>
       </c>
@@ -28109,7 +28069,7 @@
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="67" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>4</v>
       </c>
@@ -28525,7 +28485,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="68" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
         <v>4</v>
       </c>
@@ -28941,7 +28901,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="69" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
         <v>4</v>
       </c>
@@ -29357,7 +29317,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="70" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
         <v>4</v>
       </c>
@@ -29773,7 +29733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
         <v>4</v>
       </c>
@@ -30189,7 +30149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A72" s="8" t="s">
         <v>0</v>
       </c>
@@ -30605,7 +30565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
         <v>5</v>
       </c>
@@ -31021,7 +30981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
         <v>5</v>
       </c>
@@ -31437,7 +31397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
         <v>5</v>
       </c>
@@ -31853,7 +31813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
         <v>5</v>
       </c>
@@ -32269,7 +32229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
         <v>5</v>
       </c>
@@ -32685,7 +32645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
         <v>5</v>
       </c>
@@ -33101,7 +33061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
         <v>5</v>
       </c>
@@ -33517,7 +33477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
         <v>5</v>
       </c>
@@ -33933,7 +33893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
         <v>5</v>
       </c>
@@ -34349,7 +34309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
         <v>5</v>
       </c>
@@ -34765,7 +34725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
         <v>5</v>
       </c>
@@ -35181,7 +35141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
         <v>5</v>
       </c>
@@ -35597,7 +35557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
         <v>5</v>
       </c>
@@ -36013,7 +35973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
         <v>5</v>
       </c>
@@ -36429,7 +36389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
         <v>5</v>
       </c>
@@ -36845,7 +36805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
         <v>5</v>
       </c>
@@ -37261,7 +37221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
         <v>5</v>
       </c>
@@ -37677,7 +37637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
         <v>5</v>
       </c>
@@ -38093,7 +38053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
         <v>5</v>
       </c>
@@ -38509,7 +38469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
         <v>5</v>
       </c>
@@ -38925,7 +38885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
         <v>5</v>
       </c>
@@ -39341,7 +39301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
         <v>5</v>
       </c>
@@ -39757,7 +39717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
         <v>5</v>
       </c>
@@ -40173,7 +40133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
         <v>5</v>
       </c>
@@ -40589,7 +40549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
         <v>5</v>
       </c>
@@ -41005,7 +40965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
         <v>5</v>
       </c>
@@ -41421,7 +41381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
         <v>5</v>
       </c>
@@ -41837,7 +41797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
         <v>5</v>
       </c>
@@ -42253,7 +42213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
         <v>5</v>
       </c>
@@ -42669,7 +42629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
         <v>5</v>
       </c>
@@ -43085,7 +43045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A103" s="5" t="s">
         <v>5</v>
       </c>
@@ -43501,7 +43461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A104" s="5" t="s">
         <v>5</v>
       </c>
@@ -43917,7 +43877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
         <v>5</v>
       </c>
@@ -44333,7 +44293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="s">
         <v>5</v>
       </c>
@@ -44749,7 +44709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
         <v>5</v>
       </c>
@@ -45165,7 +45125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A108" s="5" t="s">
         <v>5</v>
       </c>
@@ -45581,7 +45541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A109" s="5" t="s">
         <v>5</v>
       </c>
@@ -45997,7 +45957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A110" s="5" t="s">
         <v>5</v>
       </c>
@@ -46413,7 +46373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
         <v>5</v>
       </c>
@@ -46829,7 +46789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
         <v>5</v>
       </c>
@@ -47245,7 +47205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A113" s="5" t="s">
         <v>5</v>
       </c>
@@ -47661,7 +47621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
         <v>5</v>
       </c>
@@ -48077,7 +48037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
         <v>5</v>
       </c>
@@ -48493,7 +48453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
         <v>5</v>
       </c>
@@ -48909,7 +48869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A117" s="5" t="s">
         <v>5</v>
       </c>
@@ -49325,7 +49285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A118" s="5" t="s">
         <v>5</v>
       </c>
@@ -49741,7 +49701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A119" s="5" t="s">
         <v>5</v>
       </c>
@@ -50157,7 +50117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A120" s="5" t="s">
         <v>5</v>
       </c>
@@ -50573,7 +50533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A121" s="5" t="s">
         <v>5</v>
       </c>
@@ -50989,7 +50949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
         <v>5</v>
       </c>
@@ -51405,7 +51365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A123" s="5" t="s">
         <v>5</v>
       </c>
@@ -51821,7 +51781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A124" s="5" t="s">
         <v>5</v>
       </c>
@@ -52237,7 +52197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A125" s="5" t="s">
         <v>5</v>
       </c>
@@ -52653,7 +52613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A126" s="5" t="s">
         <v>5</v>
       </c>
@@ -53069,7 +53029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A127" s="5" t="s">
         <v>5</v>
       </c>
@@ -53485,7 +53445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A128" s="5" t="s">
         <v>5</v>
       </c>
@@ -53901,7 +53861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A129" s="5" t="s">
         <v>5</v>
       </c>
@@ -54317,7 +54277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A130" s="5" t="s">
         <v>5</v>
       </c>
@@ -54733,7 +54693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A131" s="5" t="s">
         <v>5</v>
       </c>
@@ -55149,7 +55109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
         <v>5</v>
       </c>
@@ -55565,7 +55525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A133" s="5" t="s">
         <v>5</v>
       </c>
@@ -55981,7 +55941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A134" s="5" t="s">
         <v>5</v>
       </c>
@@ -56397,7 +56357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="s">
         <v>5</v>
       </c>
@@ -56813,7 +56773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A136" s="5" t="s">
         <v>5</v>
       </c>
@@ -57229,7 +57189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A137" s="5" t="s">
         <v>5</v>
       </c>
@@ -57645,7 +57605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A138" s="5" t="s">
         <v>173</v>
       </c>
@@ -58061,7 +58021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A139" s="5" t="s">
         <v>173</v>
       </c>
@@ -58477,7 +58437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A140" s="5" t="s">
         <v>173</v>
       </c>
@@ -58893,7 +58853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A141" s="5" t="s">
         <v>173</v>
       </c>
@@ -59309,7 +59269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A142" s="5" t="s">
         <v>173</v>
       </c>
@@ -59725,7 +59685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:139" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:139" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="5" t="s">
         <v>2</v>
       </c>
@@ -60141,7 +60101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A144" s="11" t="s">
         <v>164</v>
       </c>
@@ -60558,7 +60518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:148" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:148" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A145" s="11" t="s">
         <v>164</v>
       </c>
@@ -60975,7 +60935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:148" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:148" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A146" s="11" t="s">
         <v>164</v>
       </c>
@@ -61392,7 +61352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:148" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:148" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A147" s="11" t="s">
         <v>164</v>
       </c>
@@ -61809,7 +61769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:148" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:148" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A148" s="11" t="s">
         <v>164</v>
       </c>
@@ -62226,7 +62186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:148" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:148" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A149" s="11" t="s">
         <v>164</v>
       </c>
@@ -62643,7 +62603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:148" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:148" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A150" s="11" t="s">
         <v>164</v>
       </c>
@@ -63060,7 +63020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:148" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:148" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A151" s="11" t="s">
         <v>164</v>
       </c>
@@ -63477,7 +63437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:148" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A152" s="11" t="s">
         <v>164</v>
       </c>
@@ -63894,7 +63854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:148" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:148" x14ac:dyDescent="0.25">
       <c r="A153" s="11" t="s">
         <v>164</v>
       </c>
@@ -64311,7 +64271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:148" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:148" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A154" s="11" t="s">
         <v>164</v>
       </c>
@@ -64728,7 +64688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:148" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:148" ht="14.45" x14ac:dyDescent="0.3">
       <c r="F155" s="4"/>
       <c r="G155" s="4"/>
       <c r="H155" s="4"/>
@@ -64873,7 +64833,7 @@
       <c r="EQ155" s="4"/>
       <c r="ER155" s="4"/>
     </row>
-    <row r="156" spans="1:148" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:148" ht="14.45" x14ac:dyDescent="0.3">
       <c r="F156" s="4"/>
       <c r="G156" s="4"/>
       <c r="H156" s="4"/>
@@ -65018,7 +64978,7 @@
       <c r="EQ156" s="4"/>
       <c r="ER156" s="4"/>
     </row>
-    <row r="157" spans="1:148" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:148" ht="14.45" x14ac:dyDescent="0.3">
       <c r="F157" s="4"/>
       <c r="G157" s="4"/>
       <c r="H157" s="4"/>
@@ -65164,7 +65124,7 @@
       <c r="ER157" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="B7:D143" xr:uid="{12D394F5-05BD-40D2-B24B-C6B9DB90E7B7}"/>
+  <autoFilter ref="B7:D143"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>